<commit_message>
tables and figures added
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="tables" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="figures" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="23">
   <si>
     <t xml:space="preserve">MPEC</t>
   </si>
@@ -83,6 +84,12 @@
   </si>
   <si>
     <t xml:space="preserve">Cournot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OLD &gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW&gt;&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -97,6 +104,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -118,6 +126,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -189,7 +198,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -218,6 +227,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -230,6 +243,719 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>803520</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>134640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>519120</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>142560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7207920" y="2898000"/>
+          <a:ext cx="4607640" cy="3096720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>79200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>293760</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>104040</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7299000" y="337680"/>
+          <a:ext cx="4291200" cy="2692440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>29520</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>55080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>460440</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>131760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 3" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7249320" y="5907240"/>
+          <a:ext cx="4507560" cy="3002760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>17280</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>376560</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19080</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9770760" y="0"/>
+          <a:ext cx="5236200" cy="3270240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>809280</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>86400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>356760</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>105840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 5" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9749880" y="3337560"/>
+          <a:ext cx="5237280" cy="3270600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1800</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>115200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>287280</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>88200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 6" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9755280" y="6779880"/>
+          <a:ext cx="5162400" cy="3224160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>799560</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>15120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>307080</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>9720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 7" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9740160" y="10256400"/>
+          <a:ext cx="5197320" cy="3245760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>801720</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>9720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>287280</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>153000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Image 8" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9742320" y="13664520"/>
+          <a:ext cx="5175360" cy="3232080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>16920</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>38160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>330480</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>28800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Image 9" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId6"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9770400" y="17106840"/>
+          <a:ext cx="5190480" cy="3241800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>14040</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>144000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>341640</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>143280</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Image 10" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId7"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9767520" y="20626560"/>
+          <a:ext cx="5204520" cy="3250440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9720</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>57960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>398520</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>95400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Image 11" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId8"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9763200" y="24116760"/>
+          <a:ext cx="5265720" cy="3288600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>347040</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>207360</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>106920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Image 12" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId9"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1159560" y="0"/>
+          <a:ext cx="4737240" cy="3195360"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>197640</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Image 13" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId10"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="812520" y="3251160"/>
+          <a:ext cx="5074560" cy="3422880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>197640</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>9000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Image 14" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId11"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="812520" y="6827400"/>
+          <a:ext cx="5074560" cy="3422880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>153000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>197640</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>162000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Image 15" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId12"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="812520" y="10231560"/>
+          <a:ext cx="5074560" cy="3422880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>792720</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>152640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>177840</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>162000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Image 16" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId13"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="792720" y="13645080"/>
+          <a:ext cx="5074560" cy="3422880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>19440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>197640</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>28440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Image 17" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId14"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="812520" y="16925400"/>
+          <a:ext cx="5074560" cy="3422880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>197640</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>9000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Image 18" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId15"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="812520" y="20644920"/>
+          <a:ext cx="5074560" cy="3422880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19800</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>143640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>217440</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>153000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Image 19" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId16"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="832320" y="24202440"/>
+          <a:ext cx="5074560" cy="3422880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -237,11 +963,11 @@
   </sheetPr>
   <dimension ref="E3:H53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J29" activeCellId="0" sqref="J29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q7" activeCellId="0" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.44"/>
   </cols>
@@ -917,5 +1643,39 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A3:K3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K149" activeCellId="0" sqref="K149"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>